<commit_message>
修复 MiniDesignerConfigsTemplate/Datas/item.xlsx的错误 修复 ConvertTemplates/gen_convert_unity_asset.bat 错误
</commit_message>
<xml_diff>
--- a/MiniDesignerConfigsTemplate/Datas/item.xlsx
+++ b/MiniDesignerConfigsTemplate/Datas/item.xlsx
@@ -1,275 +1,391 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\luban_examples\MiniDesignerConfigsTemplate\Datas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36CCFAC-56AF-466F-9182-1BC22A2711D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="25140" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20130" windowHeight="8865"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
-    <t>int</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>名字</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>描述</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>##var</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>i</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF006100"/>
-        <rFont val="等线"/>
-        <family val="3"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>d</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>d</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF006100"/>
-        <rFont val="等线"/>
-        <family val="3"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>esc</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>upgrade_to_item_id</t>
+  </si>
+  <si>
+    <t>expire_time</t>
+  </si>
+  <si>
+    <t>batch_useable</t>
+  </si>
+  <si>
+    <t>##type</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>int#ref=item.TbItem</t>
+  </si>
+  <si>
+    <t>datetime?</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>##</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>这是i</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF006100"/>
-        <rFont val="等线"/>
-        <family val="3"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>d</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>价格</t>
+  </si>
+  <si>
+    <t>过期时间</t>
+  </si>
+  <si>
+    <t>能否批量使用</t>
   </si>
   <si>
     <t>发型</t>
   </si>
   <si>
-    <t>外套</t>
-  </si>
-  <si>
-    <t>上衣</t>
-  </si>
-  <si>
-    <t>裙子</t>
-  </si>
-  <si>
-    <t>袜子</t>
-  </si>
-  <si>
-    <t>发饰</t>
-  </si>
-  <si>
     <t>初始发型</t>
   </si>
   <si>
-    <t>初始外套</t>
-  </si>
-  <si>
-    <t>初始上衣</t>
-  </si>
-  <si>
-    <t>初始下装</t>
-  </si>
-  <si>
-    <t>初始袜子</t>
-  </si>
-  <si>
-    <t>初始鞋子</t>
-  </si>
-  <si>
-    <t>初始发饰</t>
-  </si>
-  <si>
-    <t>price</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>价格</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>expire_time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>datetime?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>中秋节发饰</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>鞋子</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>中秋节鞋子</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>n</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>ull</t>
     </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>外套</t>
+  </si>
+  <si>
+    <t>初始外套</t>
+  </si>
+  <si>
+    <t>上衣</t>
+  </si>
+  <si>
+    <t>初始上衣</t>
+  </si>
+  <si>
+    <t>裙子</t>
+  </si>
+  <si>
+    <t>初始下装</t>
+  </si>
+  <si>
+    <t>袜子</t>
+  </si>
+  <si>
+    <t>初始袜子</t>
+  </si>
+  <si>
+    <t>鞋子</t>
+  </si>
+  <si>
+    <t>初始鞋子</t>
+  </si>
+  <si>
+    <t>发饰</t>
+  </si>
+  <si>
+    <t>初始发饰</t>
+  </si>
+  <si>
+    <t>中秋节发饰</t>
+  </si>
+  <si>
+    <t>中秋节鞋子</t>
   </si>
   <si>
     <t>礼包</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>中秋节礼包</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>null</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_useable</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>能否批量使用</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>过期时间</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>upgrade_to_item_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>int&amp;ref=item.TbItem</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>##</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>##type</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>##var</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
-      <family val="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <family val="2"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,10 +401,185 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -296,36 +587,314 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="23" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="29" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="差" xfId="2" builtinId="27"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -583,114 +1152,114 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="12.25" customWidth="1"/>
-    <col min="6" max="6" width="22.375" customWidth="1"/>
-    <col min="7" max="7" width="16.875" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
+    <col min="1" max="1" width="12.5047619047619" customWidth="1"/>
+    <col min="2" max="2" width="15.8761904761905" customWidth="1"/>
+    <col min="3" max="3" width="17.8761904761905" customWidth="1"/>
+    <col min="4" max="4" width="12.3714285714286" customWidth="1"/>
+    <col min="5" max="5" width="12.247619047619" customWidth="1"/>
+    <col min="6" max="6" width="22.3714285714286" customWidth="1"/>
+    <col min="7" max="7" width="16.8761904761905" customWidth="1"/>
+    <col min="8" max="8" width="13.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>32</v>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>34</v>
+    <row r="2" s="2" customFormat="1" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>33</v>
+    <row r="3" s="1" customFormat="1" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8">
       <c r="B4">
         <v>10000</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -698,22 +1267,22 @@
       <c r="F4">
         <v>10001</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>28</v>
+      <c r="G4" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8">
       <c r="B5">
         <v>10001</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -721,22 +1290,22 @@
       <c r="F5">
         <v>10002</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
+      <c r="G5" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8">
       <c r="B6">
         <v>10002</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E6">
         <v>100</v>
@@ -744,22 +1313,22 @@
       <c r="F6">
         <v>10003</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>28</v>
+      <c r="G6" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8">
       <c r="B7">
         <v>10003</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -767,22 +1336,22 @@
       <c r="F7">
         <v>10004</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
+      <c r="G7" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8">
       <c r="B8">
         <v>10004</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -790,22 +1359,22 @@
       <c r="F8">
         <v>10005</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>28</v>
+      <c r="G8" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8">
       <c r="B9">
         <v>10005</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
+      <c r="C9" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -813,22 +1382,22 @@
       <c r="F9">
         <v>10006</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>28</v>
+      <c r="G9" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8">
       <c r="B10">
         <v>10006</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -836,22 +1405,22 @@
       <c r="F10">
         <v>10007</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>28</v>
+      <c r="G10" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8">
       <c r="B11">
         <v>10007</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
+      <c r="C11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="E11">
         <v>200</v>
@@ -860,21 +1429,21 @@
         <v>10008</v>
       </c>
       <c r="G11" s="4">
-        <v>44479.999988425923</v>
+        <v>44479.9999884259</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8">
       <c r="B12">
         <v>10008</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
+      <c r="C12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="E12">
         <v>300</v>
@@ -883,21 +1452,21 @@
         <v>10009</v>
       </c>
       <c r="G12" s="4">
-        <v>44480.999988425923</v>
+        <v>44480.9999884259</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8">
       <c r="B13">
         <v>10009</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>30</v>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -905,16 +1474,16 @@
       <c r="F13">
         <v>10000</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>31</v>
+      <c r="G13" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>